<commit_message>
results for 1b generated. Excel file not pushed due to error
</commit_message>
<xml_diff>
--- a/p3-results.xlsx
+++ b/p3-results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://quinnipiacuniversity-my.sharepoint.com/personal/bconeill_quinnipiac_edu/Documents/Documents/CSC 350-500 AI/Projects/Project 3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cheff\Downloads\School_Downloads\CSC350\Project3\Clustering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="36" documentId="8_{6D7F0FA9-3B6F-4247-966F-E9988896F06E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6343AFF2-75D7-4204-8878-01C869DB64C7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B070A8A-9AE7-4EB1-8CAD-232FF1FFA909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{FF08A997-3A99-4B2C-BEDC-14A11E32874A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FF08A997-3A99-4B2C-BEDC-14A11E32874A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -534,19 +534,19 @@
   <dimension ref="A1:Q24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="11.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="8.7265625" style="2"/>
+    <col min="2" max="4" width="11.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="8.77734375" style="2"/>
     <col min="8" max="8" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="17" width="8.7265625" style="2"/>
+    <col min="9" max="17" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B1" s="6" t="s">
         <v>28</v>
       </c>
@@ -568,7 +568,7 @@
       <c r="P1" s="6"/>
       <c r="Q1" s="6"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -615,290 +615,488 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="2" t="e">
+      <c r="B3" s="2">
+        <v>22.384620000000002</v>
+      </c>
+      <c r="C3" s="2">
+        <v>22.384620000000002</v>
+      </c>
+      <c r="D3" s="2">
+        <v>22.429427</v>
+      </c>
+      <c r="E3" s="2">
         <f>MEDIAN(B3:D3)</f>
-        <v>#NUM!</v>
+        <v>22.384620000000002</v>
       </c>
       <c r="F3" s="2">
         <f>MIN(B3:D3)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+        <v>22.384620000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="2" t="e">
+      <c r="B4" s="2">
+        <v>9.7972490000000008</v>
+      </c>
+      <c r="C4" s="2">
+        <v>9.7972490000000008</v>
+      </c>
+      <c r="D4" s="2">
+        <v>9.7972490000000008</v>
+      </c>
+      <c r="E4" s="2">
         <f t="shared" ref="E4:E24" si="0">MEDIAN(B4:D4)</f>
-        <v>#NUM!</v>
+        <v>9.7972490000000008</v>
       </c>
       <c r="F4" s="2">
         <f t="shared" ref="F4:F24" si="1">MIN(B4:D4)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+        <v>9.7972490000000008</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#NUM!</v>
+      <c r="B5" s="2">
+        <v>1.1214090000000001</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1.1214090000000001</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1.1214090000000001</v>
+      </c>
+      <c r="E5" s="2">
+        <f t="shared" si="0"/>
+        <v>1.1214090000000001</v>
       </c>
       <c r="F5" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+        <v>1.1214090000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#NUM!</v>
+      <c r="B6" s="2">
+        <v>1.57145</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.52234700000000001</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1.415432</v>
+      </c>
+      <c r="E6" s="2">
+        <f t="shared" si="0"/>
+        <v>1.415432</v>
       </c>
       <c r="F6" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+        <v>0.52234700000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#NUM!</v>
+      <c r="B7" s="2">
+        <v>0.55971700000000002</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.55971700000000002</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.55971700000000002</v>
+      </c>
+      <c r="E7" s="2">
+        <f t="shared" si="0"/>
+        <v>0.55971700000000002</v>
       </c>
       <c r="F7" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+        <v>0.55971700000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#NUM!</v>
+      <c r="B8" s="2">
+        <v>0.51026800000000005</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.51026800000000005</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.51026800000000005</v>
+      </c>
+      <c r="E8" s="2">
+        <f t="shared" si="0"/>
+        <v>0.51026800000000005</v>
       </c>
       <c r="F8" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+        <v>0.51026800000000005</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#NUM!</v>
+      <c r="B9" s="2">
+        <v>0.47006199999999998</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.47006199999999998</v>
+      </c>
+      <c r="D9" s="2">
+        <v>5.2599099999999996</v>
+      </c>
+      <c r="E9" s="2">
+        <f t="shared" si="0"/>
+        <v>0.47006199999999998</v>
       </c>
       <c r="F9" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+        <v>0.47006199999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#NUM!</v>
+      <c r="B10" s="2">
+        <v>5.2264080000000002</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.51057200000000003</v>
+      </c>
+      <c r="D10" s="2">
+        <v>2.2968929999999999</v>
+      </c>
+      <c r="E10" s="2">
+        <f t="shared" si="0"/>
+        <v>2.2968929999999999</v>
       </c>
       <c r="F10" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+        <v>0.51057200000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#NUM!</v>
+      <c r="B11" s="2">
+        <v>0.46304099999999998</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1.467179</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1.4309719999999999</v>
+      </c>
+      <c r="E11" s="2">
+        <f t="shared" si="0"/>
+        <v>1.4309719999999999</v>
       </c>
       <c r="F11" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+        <v>0.46304099999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#NUM!</v>
+      <c r="B12" s="2">
+        <v>0.45367499999999999</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1.1419649999999999</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1.915395</v>
+      </c>
+      <c r="E12" s="2">
+        <f t="shared" si="0"/>
+        <v>1.1419649999999999</v>
       </c>
       <c r="F12" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+        <v>0.45367499999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#NUM!</v>
+      <c r="B13" s="2">
+        <v>0.35351399999999999</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1.394776</v>
+      </c>
+      <c r="D13" s="2">
+        <v>1.284923</v>
+      </c>
+      <c r="E13" s="2">
+        <f t="shared" si="0"/>
+        <v>1.284923</v>
       </c>
       <c r="F13" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+        <v>0.35351399999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#NUM!</v>
+      <c r="B14" s="2">
+        <v>0.79840100000000003</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.84431</v>
+      </c>
+      <c r="D14" s="2">
+        <v>1.1895690000000001</v>
+      </c>
+      <c r="E14" s="2">
+        <f t="shared" si="0"/>
+        <v>0.84431</v>
       </c>
       <c r="F14" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+        <v>0.79840100000000003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#NUM!</v>
+      <c r="B15" s="2">
+        <v>0.53415400000000002</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0.81103999999999998</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0.57713199999999998</v>
+      </c>
+      <c r="E15" s="2">
+        <f t="shared" si="0"/>
+        <v>0.57713199999999998</v>
       </c>
       <c r="F15" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+        <v>0.53415400000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#NUM!</v>
+      <c r="B16" s="2">
+        <v>0.54217000000000004</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0.54217000000000004</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0.54217000000000004</v>
+      </c>
+      <c r="E16" s="2">
+        <f t="shared" si="0"/>
+        <v>0.54217000000000004</v>
       </c>
       <c r="F16" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+        <v>0.54217000000000004</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>20</v>
       </c>
-      <c r="E17" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#NUM!</v>
+      <c r="B17" s="2">
+        <v>0.420101</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0.420101</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0.42719400000000002</v>
+      </c>
+      <c r="E17" s="2">
+        <f t="shared" si="0"/>
+        <v>0.420101</v>
       </c>
       <c r="F17" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+        <v>0.420101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>21</v>
       </c>
-      <c r="E18" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#NUM!</v>
+      <c r="B18" s="2">
+        <v>0.39005699999999999</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.41220800000000002</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.410082</v>
+      </c>
+      <c r="E18" s="2">
+        <f t="shared" si="0"/>
+        <v>0.410082</v>
       </c>
       <c r="F18" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+        <v>0.39005699999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>22</v>
       </c>
-      <c r="E19" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#NUM!</v>
+      <c r="B19" s="2">
+        <v>0.43096000000000001</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0.430338</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0.52908299999999997</v>
+      </c>
+      <c r="E19" s="2">
+        <f t="shared" si="0"/>
+        <v>0.43096000000000001</v>
       </c>
       <c r="F19" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+        <v>0.430338</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>23</v>
       </c>
-      <c r="E20" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#NUM!</v>
+      <c r="B20" s="2">
+        <v>0.434722</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0.434722</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0.53455900000000001</v>
+      </c>
+      <c r="E20" s="2">
+        <f t="shared" si="0"/>
+        <v>0.434722</v>
       </c>
       <c r="F20" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+        <v>0.434722</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>24</v>
       </c>
-      <c r="E21" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#NUM!</v>
+      <c r="B21" s="2">
+        <v>0.37440699999999999</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0.39099200000000001</v>
+      </c>
+      <c r="D21" s="2">
+        <v>0.391461</v>
+      </c>
+      <c r="E21" s="2">
+        <f t="shared" si="0"/>
+        <v>0.39099200000000001</v>
       </c>
       <c r="F21" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+        <v>0.37440699999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>25</v>
       </c>
-      <c r="E22" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#NUM!</v>
+      <c r="B22" s="2">
+        <v>0.33624700000000002</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0.33172200000000002</v>
+      </c>
+      <c r="D22" s="2">
+        <v>0.36504900000000001</v>
+      </c>
+      <c r="E22" s="2">
+        <f t="shared" si="0"/>
+        <v>0.33624700000000002</v>
       </c>
       <c r="F22" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+        <v>0.33172200000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>26</v>
       </c>
-      <c r="E23" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#NUM!</v>
+      <c r="B23" s="2">
+        <v>0.40323900000000001</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0.35052499999999998</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0.37901499999999999</v>
+      </c>
+      <c r="E23" s="2">
+        <f t="shared" si="0"/>
+        <v>0.37901499999999999</v>
       </c>
       <c r="F23" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+        <v>0.35052499999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>27</v>
       </c>
-      <c r="E24" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#NUM!</v>
+      <c r="B24" s="2">
+        <v>1.258313</v>
+      </c>
+      <c r="C24" s="2">
+        <v>1.258313</v>
+      </c>
+      <c r="D24" s="2">
+        <v>1.258313</v>
+      </c>
+      <c r="E24" s="2">
+        <f t="shared" si="0"/>
+        <v>1.258313</v>
       </c>
       <c r="F24" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.258313</v>
       </c>
     </row>
   </sheetData>

</xml_diff>